<commit_message>
added automatic detection and conversion to NaN of values out of rang…
</commit_message>
<xml_diff>
--- a/src/Sprint 1/FeatureListe.xlsx
+++ b/src/Sprint 1/FeatureListe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angst\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbene\Air-regression\src\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C149B5EA-BEBC-4092-819B-11552F8199F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1222276-AE51-41BE-82B9-6FF4B815579C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="910" windowWidth="17970" windowHeight="8700" xr2:uid="{0F794381-D9F4-4A68-87A1-3B277EA5ED33}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{0F794381-D9F4-4A68-87A1-3B277EA5ED33}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -182,13 +182,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="00.000000"/>
-    <numFmt numFmtId="173" formatCode="0000.000000"/>
-    <numFmt numFmtId="175" formatCode="00.0000000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -248,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,24 +252,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -593,7 +577,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,10 +638,10 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>0.1</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>11.9</v>
       </c>
       <c r="E3" t="s">
@@ -672,10 +656,10 @@
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="8">
         <v>647</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>2040</v>
       </c>
       <c r="H4" s="1"/>
@@ -687,10 +671,10 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>7</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>1189</v>
       </c>
       <c r="E5" t="s">
@@ -705,10 +689,10 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>0.1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>63.7</v>
       </c>
       <c r="E6" t="s">
@@ -723,10 +707,10 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="8">
         <v>383</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>2214</v>
       </c>
       <c r="H7" s="1"/>
@@ -738,10 +722,10 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>2</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>1479</v>
       </c>
       <c r="H8" s="1"/>
@@ -753,10 +737,10 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="8">
         <v>322</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="7">
         <v>2683</v>
       </c>
       <c r="H9" s="1"/>
@@ -768,10 +752,10 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>2</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="E10" t="s">
@@ -786,10 +770,10 @@
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="8">
         <v>657</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>2775</v>
       </c>
       <c r="H11" s="1"/>
@@ -801,10 +785,10 @@
       <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="8">
         <v>253</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H12" s="1"/>
@@ -816,10 +800,10 @@
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <v>0.3</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>44.6</v>
       </c>
       <c r="E13" t="s">
@@ -834,10 +818,10 @@
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <v>88.7</v>
       </c>
       <c r="E14" t="s">
@@ -852,10 +836,10 @@
       <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="8">
         <v>0.1988</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="6">
         <v>2231</v>
       </c>
       <c r="H15" s="1"/>

</xml_diff>